<commit_message>
Se actualizan los cambios
</commit_message>
<xml_diff>
--- a/Documents/Actividades realizadas/ActividadesN.xlsx
+++ b/Documents/Actividades realizadas/ActividadesN.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Cotización vs Real" sheetId="2" r:id="rId2"/>
+    <sheet name="Pendientes" sheetId="3" r:id="rId2"/>
+    <sheet name="Cotización vs Real" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="555" uniqueCount="263">
   <si>
     <t>Descripción</t>
   </si>
@@ -721,6 +722,105 @@
   </si>
   <si>
     <t>Conexiones de soporte</t>
+  </si>
+  <si>
+    <t>Revisiones de redondeo</t>
+  </si>
+  <si>
+    <t>Verificación de inventario por selección</t>
+  </si>
+  <si>
+    <t>Hrs Estimadas</t>
+  </si>
+  <si>
+    <t>Hrs Reales</t>
+  </si>
+  <si>
+    <t>Ventana</t>
+  </si>
+  <si>
+    <t>Corte de caja</t>
+  </si>
+  <si>
+    <t>PONER LAS VENTAS DE TALLER APARTE</t>
+  </si>
+  <si>
+    <t>Estatus</t>
+  </si>
+  <si>
+    <t>COMPLETO</t>
+  </si>
+  <si>
+    <t>PERMISO DE CAMBIOS EN SOBRE DE TALLER</t>
+  </si>
+  <si>
+    <t>VENTAS</t>
+  </si>
+  <si>
+    <t>Cambio de permiso en actualización de sobre</t>
+  </si>
+  <si>
+    <t>PONER PRECIO Y COSTO PERO NOMAS A MARTIN (PERMISO PERSONALIZADO)</t>
+  </si>
+  <si>
+    <t>TODO</t>
+  </si>
+  <si>
+    <t>HACER EGRESO DE DOLARES TAMBIEN</t>
+  </si>
+  <si>
+    <t>EGRESOS</t>
+  </si>
+  <si>
+    <t>incidente con el corte de caja que no sumaba si no le dabas hasta el final</t>
+  </si>
+  <si>
+    <t>PONER LAS VENTAS DE TALLER APARTE Y CAMBIAR LOS REPORTES DE CORTES DE CAJA</t>
+  </si>
+  <si>
+    <t>Se agrega Ingreso real en el corte de Caja y en loas Cortes Historicos</t>
+  </si>
+  <si>
+    <t>Reporte de ventas</t>
+  </si>
+  <si>
+    <t>Regla para que las notas de consignación para Martín pida autorización</t>
+  </si>
+  <si>
+    <t>Configuración e instalación de impresora en mostrador</t>
+  </si>
+  <si>
+    <t>Agregar descuento por dinero</t>
+  </si>
+  <si>
+    <t>Crear la devolución de inventario</t>
+  </si>
+  <si>
+    <t>Inventario</t>
+  </si>
+  <si>
+    <t>Agregar el descuento pero en pesos en la pantalla de ventas, solucionar detalle de los decimales en los pagos</t>
+  </si>
+  <si>
+    <t>Mostrar Log de quien autoriza las cosas</t>
+  </si>
+  <si>
+    <t>Devolución de inventarios</t>
+  </si>
+  <si>
+    <t>Agregar una nota de entrada de inventario que sumarice el costo</t>
+  </si>
+  <si>
+    <t>Agregar margen de 30% despues del costo para los descuentos</t>
+  </si>
+  <si>
+    <t>Agregar cambio de precio y con permiso</t>
+  </si>
+  <si>
+    <t>Al agregar descuento por precio, agregar alerta de si está seguro</t>
+  </si>
+  <si>
+    <t>Rediseñar impresión de ticket de taller notas de taller</t>
   </si>
 </sst>
 </file>
@@ -789,7 +889,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -838,6 +938,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -853,7 +959,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -921,6 +1027,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="43" fontId="7" fillId="6" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="44" fontId="3" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1291,11 +1406,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K257"/>
+  <dimension ref="A1:K267"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A199" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A213" sqref="A213"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A214" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G222" sqref="G222:G223"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5498,7 +5613,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="209" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A209" s="5">
         <v>45345</v>
       </c>
@@ -5515,7 +5630,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="210" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A210" s="5">
         <v>45346</v>
       </c>
@@ -5532,7 +5647,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="211" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A211" s="5">
         <v>45346</v>
       </c>
@@ -5549,7 +5664,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="212" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A212" s="5">
         <v>45346</v>
       </c>
@@ -5566,7 +5681,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="213" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A213" s="5"/>
       <c r="D213" t="s">
         <v>229</v>
@@ -5581,294 +5696,364 @@
         <v>2</v>
       </c>
     </row>
-    <row r="214" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A214" s="5"/>
-      <c r="E214" s="2"/>
-      <c r="F214" s="2"/>
-    </row>
-    <row r="215" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D214" t="s">
+        <v>230</v>
+      </c>
+      <c r="E214" s="2">
+        <v>0.375</v>
+      </c>
+      <c r="F214" s="2">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="G214" s="15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="215" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A215" s="5"/>
-      <c r="E215" s="2"/>
-      <c r="F215" s="2"/>
-    </row>
-    <row r="216" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D215" t="s">
+        <v>231</v>
+      </c>
+      <c r="E215" s="2">
+        <v>0.375</v>
+      </c>
+      <c r="F215" s="2">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="G215" s="15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="216" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A216" s="5"/>
-      <c r="E216" s="2"/>
-      <c r="F216" s="2"/>
-    </row>
-    <row r="217" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D216" t="s">
+        <v>241</v>
+      </c>
+      <c r="E216" s="2">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="F216" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="G216" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="217" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A217" s="5"/>
-      <c r="E217" s="2"/>
-      <c r="F217" s="2"/>
-    </row>
-    <row r="218" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A218" s="47" t="s">
+      <c r="D217" s="14" t="s">
+        <v>247</v>
+      </c>
+      <c r="E217" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="F217" s="2">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="G217" s="15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="218" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A218" s="5"/>
+      <c r="D218" t="s">
+        <v>248</v>
+      </c>
+      <c r="E218" s="2">
+        <v>0.375</v>
+      </c>
+      <c r="F218" s="2">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="G218" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="219" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A219" s="5"/>
+      <c r="D219" t="s">
+        <v>249</v>
+      </c>
+      <c r="E219" s="2">
+        <v>0.375</v>
+      </c>
+      <c r="F219" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="G219" s="15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="220" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A220" s="5"/>
+      <c r="D220" t="s">
+        <v>250</v>
+      </c>
+      <c r="E220" s="2">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="F220" s="2">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="G220" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="221" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A221" s="5"/>
+      <c r="D221" t="s">
+        <v>251</v>
+      </c>
+      <c r="E221" s="2">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="F221" s="2">
+        <v>0.20833333333333334</v>
+      </c>
+      <c r="H221" s="15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="222" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A222" s="5"/>
+      <c r="D222" s="14" t="s">
+        <v>255</v>
+      </c>
+      <c r="E222" s="2">
+        <v>0.375</v>
+      </c>
+      <c r="F222" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="G222" s="15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="223" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A223" s="5"/>
+      <c r="D223" t="s">
+        <v>257</v>
+      </c>
+      <c r="E223" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="F223" s="2">
+        <v>0.20833333333333334</v>
+      </c>
+      <c r="G223" s="15">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="224" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A224" s="5"/>
+      <c r="E224" s="2"/>
+      <c r="F224" s="2"/>
+    </row>
+    <row r="225" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A225" s="5"/>
+      <c r="E225" s="2"/>
+      <c r="F225" s="2"/>
+    </row>
+    <row r="226" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A226" s="5"/>
+      <c r="E226" s="2"/>
+      <c r="F226" s="2"/>
+    </row>
+    <row r="227" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A227" s="5"/>
+      <c r="E227" s="2"/>
+      <c r="F227" s="2"/>
+    </row>
+    <row r="228" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A228" s="50" t="s">
         <v>165</v>
       </c>
-      <c r="B218" s="47"/>
-      <c r="C218" s="47"/>
-      <c r="D218" s="47"/>
-      <c r="E218" s="47"/>
-      <c r="F218" s="47"/>
-      <c r="G218" s="17">
-        <f>SUM(G2:G217)</f>
-        <v>217.78999999999994</v>
-      </c>
-      <c r="H218" s="17">
-        <f>SUM(H2:H217)</f>
-        <v>38.799999999999997</v>
-      </c>
-    </row>
-    <row r="219" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A219" s="47" t="s">
+      <c r="B228" s="50"/>
+      <c r="C228" s="50"/>
+      <c r="D228" s="50"/>
+      <c r="E228" s="50"/>
+      <c r="F228" s="50"/>
+      <c r="G228" s="17">
+        <f>SUM(G2:G227)</f>
+        <v>238.78999999999994</v>
+      </c>
+      <c r="H228" s="17">
+        <f>SUM(H2:H227)</f>
+        <v>42.8</v>
+      </c>
+    </row>
+    <row r="229" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A229" s="50" t="s">
         <v>139</v>
       </c>
-      <c r="B219" s="47"/>
-      <c r="C219" s="47"/>
-      <c r="D219" s="47"/>
-      <c r="E219" s="47"/>
-      <c r="F219" s="47"/>
-      <c r="G219" s="17">
+      <c r="B229" s="50"/>
+      <c r="C229" s="50"/>
+      <c r="D229" s="50"/>
+      <c r="E229" s="50"/>
+      <c r="F229" s="50"/>
+      <c r="G229" s="17">
         <v>200</v>
       </c>
-      <c r="H219" s="17">
+      <c r="H229" s="17">
         <v>300</v>
       </c>
     </row>
-    <row r="220" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A220" s="47" t="s">
+    <row r="230" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A230" s="50" t="s">
         <v>166</v>
       </c>
-      <c r="B220" s="47"/>
-      <c r="C220" s="47"/>
-      <c r="D220" s="47"/>
-      <c r="E220" s="47"/>
-      <c r="F220" s="47"/>
-      <c r="G220" s="18">
-        <f>G219*G218</f>
-        <v>43557.999999999985</v>
-      </c>
-      <c r="H220" s="19">
-        <f>H219*H218</f>
-        <v>11640</v>
-      </c>
-      <c r="J220">
+      <c r="B230" s="50"/>
+      <c r="C230" s="50"/>
+      <c r="D230" s="50"/>
+      <c r="E230" s="50"/>
+      <c r="F230" s="50"/>
+      <c r="G230" s="18">
+        <f>G229*G228</f>
+        <v>47757.999999999985</v>
+      </c>
+      <c r="H230" s="19">
+        <f>H229*H228</f>
+        <v>12840</v>
+      </c>
+      <c r="J230">
         <v>-500</v>
       </c>
     </row>
-    <row r="221" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A221" s="47" t="s">
+    <row r="231" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A231" s="50" t="s">
         <v>140</v>
       </c>
-      <c r="B221" s="47"/>
-      <c r="C221" s="47"/>
-      <c r="D221" s="47"/>
-      <c r="E221" s="47"/>
-      <c r="F221" s="47"/>
-      <c r="G221" s="35">
-        <f>G220+H220</f>
-        <v>55197.999999999985</v>
-      </c>
-      <c r="H221" s="35"/>
-    </row>
-    <row r="222" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A222" s="11"/>
-      <c r="B222" s="38" t="s">
+      <c r="B231" s="50"/>
+      <c r="C231" s="50"/>
+      <c r="D231" s="50"/>
+      <c r="E231" s="50"/>
+      <c r="F231" s="50"/>
+      <c r="G231" s="38">
+        <f>G230+H230</f>
+        <v>60597.999999999985</v>
+      </c>
+      <c r="H231" s="38"/>
+    </row>
+    <row r="232" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A232" s="11"/>
+      <c r="B232" s="41" t="s">
         <v>142</v>
       </c>
-      <c r="C222" s="38"/>
-      <c r="D222" s="38"/>
-      <c r="E222" s="38"/>
-      <c r="F222" s="38"/>
-      <c r="G222" s="22"/>
-    </row>
-    <row r="223" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A223" s="12">
+      <c r="C232" s="41"/>
+      <c r="D232" s="41"/>
+      <c r="E232" s="41"/>
+      <c r="F232" s="41"/>
+      <c r="G232" s="22"/>
+    </row>
+    <row r="233" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A233" s="12">
         <v>45109</v>
       </c>
-      <c r="B223" s="39" t="s">
+      <c r="B233" s="42" t="s">
         <v>141</v>
       </c>
-      <c r="C223" s="39"/>
-      <c r="D223" s="39"/>
-      <c r="E223" s="39"/>
-      <c r="F223" s="39"/>
-      <c r="G223" s="41">
+      <c r="C233" s="42"/>
+      <c r="D233" s="42"/>
+      <c r="E233" s="42"/>
+      <c r="F233" s="42"/>
+      <c r="G233" s="44">
         <v>10000</v>
       </c>
-      <c r="H223" s="41"/>
-    </row>
-    <row r="224" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A224" s="12"/>
-      <c r="B224" s="43" t="s">
+      <c r="H233" s="44"/>
+    </row>
+    <row r="234" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A234" s="12"/>
+      <c r="B234" s="46" t="s">
         <v>178</v>
       </c>
-      <c r="C224" s="43"/>
-      <c r="D224" s="43"/>
-      <c r="E224" s="43"/>
-      <c r="F224" s="43"/>
-      <c r="G224" s="41">
+      <c r="C234" s="46"/>
+      <c r="D234" s="46"/>
+      <c r="E234" s="46"/>
+      <c r="F234" s="46"/>
+      <c r="G234" s="44">
         <v>5000</v>
       </c>
-      <c r="H224" s="41"/>
-    </row>
-    <row r="225" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A225" s="12">
+      <c r="H234" s="44"/>
+    </row>
+    <row r="235" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A235" s="12">
         <v>45278</v>
       </c>
-      <c r="B225" s="40" t="s">
+      <c r="B235" s="43" t="s">
         <v>178</v>
       </c>
-      <c r="C225" s="40"/>
-      <c r="D225" s="40"/>
-      <c r="E225" s="40"/>
-      <c r="F225" s="40"/>
-      <c r="G225" s="41">
+      <c r="C235" s="43"/>
+      <c r="D235" s="43"/>
+      <c r="E235" s="43"/>
+      <c r="F235" s="43"/>
+      <c r="G235" s="44">
         <v>9800</v>
       </c>
-      <c r="H225" s="41"/>
-    </row>
-    <row r="226" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A226" s="12"/>
-      <c r="B226" s="40"/>
-      <c r="C226" s="40"/>
-      <c r="D226" s="40"/>
-      <c r="E226" s="40"/>
-      <c r="F226" s="40"/>
-      <c r="G226" s="42"/>
-      <c r="H226" s="42"/>
-    </row>
-    <row r="227" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A227" s="12"/>
-      <c r="B227" s="40"/>
-      <c r="C227" s="40"/>
-      <c r="D227" s="40"/>
-      <c r="E227" s="40"/>
-      <c r="F227" s="40"/>
-      <c r="G227" s="42"/>
-      <c r="H227" s="42"/>
-    </row>
-    <row r="228" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A228" s="12"/>
-      <c r="B228" s="40"/>
-      <c r="C228" s="40"/>
-      <c r="D228" s="40"/>
-      <c r="E228" s="40"/>
-      <c r="F228" s="40"/>
-      <c r="G228" s="42"/>
-      <c r="H228" s="42"/>
-    </row>
-    <row r="229" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A229" s="12"/>
-      <c r="B229" s="40" t="s">
+      <c r="H235" s="44"/>
+    </row>
+    <row r="236" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A236" s="12"/>
+      <c r="B236" s="43"/>
+      <c r="C236" s="43"/>
+      <c r="D236" s="43"/>
+      <c r="E236" s="43"/>
+      <c r="F236" s="43"/>
+      <c r="G236" s="45"/>
+      <c r="H236" s="45"/>
+    </row>
+    <row r="237" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A237" s="12"/>
+      <c r="B237" s="43"/>
+      <c r="C237" s="43"/>
+      <c r="D237" s="43"/>
+      <c r="E237" s="43"/>
+      <c r="F237" s="43"/>
+      <c r="G237" s="45"/>
+      <c r="H237" s="45"/>
+    </row>
+    <row r="238" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A238" s="12"/>
+      <c r="B238" s="43"/>
+      <c r="C238" s="43"/>
+      <c r="D238" s="43"/>
+      <c r="E238" s="43"/>
+      <c r="F238" s="43"/>
+      <c r="G238" s="45"/>
+      <c r="H238" s="45"/>
+    </row>
+    <row r="239" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A239" s="12"/>
+      <c r="B239" s="43" t="s">
         <v>144</v>
       </c>
-      <c r="C229" s="40"/>
-      <c r="D229" s="40"/>
-      <c r="E229" s="40"/>
-      <c r="F229" s="40"/>
-      <c r="G229" s="41">
-        <f>SUM(G223:H228)</f>
+      <c r="C239" s="43"/>
+      <c r="D239" s="43"/>
+      <c r="E239" s="43"/>
+      <c r="F239" s="43"/>
+      <c r="G239" s="44">
+        <f>SUM(G233:H238)</f>
         <v>24800</v>
       </c>
-      <c r="H229" s="41"/>
-    </row>
-    <row r="230" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A230" s="36" t="s">
+      <c r="H239" s="44"/>
+    </row>
+    <row r="240" spans="1:10" ht="31.5" x14ac:dyDescent="0.5">
+      <c r="A240" s="39" t="s">
         <v>143</v>
       </c>
-      <c r="B230" s="36"/>
-      <c r="C230" s="36"/>
-      <c r="D230" s="36"/>
-      <c r="E230" s="36"/>
-      <c r="F230" s="36"/>
-      <c r="G230" s="37">
-        <f>G221-G229</f>
-        <v>30397.999999999985</v>
-      </c>
-      <c r="H230" s="37"/>
-    </row>
-    <row r="231" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A231" s="12"/>
-      <c r="B231" s="13"/>
-      <c r="C231" s="13"/>
-      <c r="D231" s="13"/>
-      <c r="E231" s="13"/>
-      <c r="F231" s="13"/>
-    </row>
-    <row r="232" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A232" s="12"/>
-      <c r="B232" s="13"/>
-      <c r="C232" s="13"/>
-      <c r="D232" s="13"/>
-      <c r="E232" s="13"/>
-      <c r="F232" s="13"/>
-    </row>
-    <row r="233" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A233" s="12"/>
-      <c r="B233" s="13"/>
-      <c r="C233" s="13"/>
-      <c r="D233" s="13"/>
-      <c r="E233" s="13"/>
-      <c r="F233" s="13"/>
-    </row>
-    <row r="234" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A234" s="12"/>
-      <c r="B234" s="13"/>
-      <c r="C234" s="13"/>
-      <c r="D234" s="13"/>
-      <c r="E234" s="13"/>
-      <c r="F234" s="13"/>
-    </row>
-    <row r="235" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A235" s="12"/>
-      <c r="B235" s="13"/>
-      <c r="C235" s="13"/>
-      <c r="D235" s="13"/>
-      <c r="E235" s="13"/>
-      <c r="F235" s="13"/>
-    </row>
-    <row r="236" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A236" s="12"/>
-      <c r="B236" s="13"/>
-      <c r="C236" s="13"/>
-      <c r="D236" s="13"/>
-      <c r="E236" s="13"/>
-      <c r="F236" s="13"/>
-    </row>
-    <row r="237" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A237" s="12"/>
-      <c r="B237" s="13"/>
-      <c r="C237" s="13"/>
-      <c r="D237" s="13"/>
-      <c r="E237" s="13"/>
-      <c r="F237" s="13"/>
-    </row>
-    <row r="238" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A238" s="12"/>
-      <c r="B238" s="13"/>
-      <c r="C238" s="13"/>
-      <c r="D238" s="13"/>
-      <c r="E238" s="13"/>
-      <c r="F238" s="13"/>
-    </row>
-    <row r="239" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A239" s="12"/>
-      <c r="B239" s="13"/>
-      <c r="C239" s="13"/>
-      <c r="D239" s="13"/>
-      <c r="E239" s="13"/>
-      <c r="F239" s="13"/>
-    </row>
-    <row r="240" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A240" s="12"/>
-      <c r="B240" s="13"/>
-      <c r="C240" s="13"/>
-      <c r="D240" s="13"/>
-      <c r="E240" s="13"/>
-      <c r="F240" s="13"/>
-    </row>
-    <row r="241" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B240" s="39"/>
+      <c r="C240" s="39"/>
+      <c r="D240" s="39"/>
+      <c r="E240" s="39"/>
+      <c r="F240" s="39"/>
+      <c r="G240" s="40">
+        <f>G231-G239</f>
+        <v>35797.999999999985</v>
+      </c>
+      <c r="H240" s="40"/>
+    </row>
+    <row r="241" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A241" s="12"/>
       <c r="B241" s="13"/>
       <c r="C241" s="13"/>
@@ -5876,7 +6061,7 @@
       <c r="E241" s="13"/>
       <c r="F241" s="13"/>
     </row>
-    <row r="242" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A242" s="12"/>
       <c r="B242" s="13"/>
       <c r="C242" s="13"/>
@@ -5884,7 +6069,7 @@
       <c r="E242" s="13"/>
       <c r="F242" s="13"/>
     </row>
-    <row r="243" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A243" s="12"/>
       <c r="B243" s="13"/>
       <c r="C243" s="13"/>
@@ -5892,7 +6077,7 @@
       <c r="E243" s="13"/>
       <c r="F243" s="13"/>
     </row>
-    <row r="244" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A244" s="12"/>
       <c r="B244" s="13"/>
       <c r="C244" s="13"/>
@@ -5900,7 +6085,7 @@
       <c r="E244" s="13"/>
       <c r="F244" s="13"/>
     </row>
-    <row r="245" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A245" s="12"/>
       <c r="B245" s="13"/>
       <c r="C245" s="13"/>
@@ -5908,7 +6093,7 @@
       <c r="E245" s="13"/>
       <c r="F245" s="13"/>
     </row>
-    <row r="246" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A246" s="12"/>
       <c r="B246" s="13"/>
       <c r="C246" s="13"/>
@@ -5916,7 +6101,7 @@
       <c r="E246" s="13"/>
       <c r="F246" s="13"/>
     </row>
-    <row r="247" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A247" s="12"/>
       <c r="B247" s="13"/>
       <c r="C247" s="13"/>
@@ -5924,7 +6109,7 @@
       <c r="E247" s="13"/>
       <c r="F247" s="13"/>
     </row>
-    <row r="248" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A248" s="12"/>
       <c r="B248" s="13"/>
       <c r="C248" s="13"/>
@@ -5932,191 +6117,271 @@
       <c r="E248" s="13"/>
       <c r="F248" s="13"/>
     </row>
-    <row r="249" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A249" s="10"/>
-      <c r="B249" s="48" t="s">
+    <row r="249" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A249" s="12"/>
+      <c r="B249" s="13"/>
+      <c r="C249" s="13"/>
+      <c r="D249" s="13"/>
+      <c r="E249" s="13"/>
+      <c r="F249" s="13"/>
+    </row>
+    <row r="250" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A250" s="12"/>
+      <c r="B250" s="13"/>
+      <c r="C250" s="13"/>
+      <c r="D250" s="13"/>
+      <c r="E250" s="13"/>
+      <c r="F250" s="13"/>
+    </row>
+    <row r="251" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A251" s="12"/>
+      <c r="B251" s="13"/>
+      <c r="C251" s="13"/>
+      <c r="D251" s="13"/>
+      <c r="E251" s="13"/>
+      <c r="F251" s="13"/>
+    </row>
+    <row r="252" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A252" s="12"/>
+      <c r="B252" s="13"/>
+      <c r="C252" s="13"/>
+      <c r="D252" s="13"/>
+      <c r="E252" s="13"/>
+      <c r="F252" s="13"/>
+    </row>
+    <row r="253" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A253" s="12"/>
+      <c r="B253" s="13"/>
+      <c r="C253" s="13"/>
+      <c r="D253" s="13"/>
+      <c r="E253" s="13"/>
+      <c r="F253" s="13"/>
+    </row>
+    <row r="254" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A254" s="12"/>
+      <c r="B254" s="13"/>
+      <c r="C254" s="13"/>
+      <c r="D254" s="13"/>
+      <c r="E254" s="13"/>
+      <c r="F254" s="13"/>
+    </row>
+    <row r="255" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A255" s="12"/>
+      <c r="B255" s="13"/>
+      <c r="C255" s="13"/>
+      <c r="D255" s="13"/>
+      <c r="E255" s="13"/>
+      <c r="F255" s="13"/>
+    </row>
+    <row r="256" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A256" s="12"/>
+      <c r="B256" s="13"/>
+      <c r="C256" s="13"/>
+      <c r="D256" s="13"/>
+      <c r="E256" s="13"/>
+      <c r="F256" s="13"/>
+    </row>
+    <row r="257" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A257" s="12"/>
+      <c r="B257" s="13"/>
+      <c r="C257" s="13"/>
+      <c r="D257" s="13"/>
+      <c r="E257" s="13"/>
+      <c r="F257" s="13"/>
+    </row>
+    <row r="258" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A258" s="12"/>
+      <c r="B258" s="13"/>
+      <c r="C258" s="13"/>
+      <c r="D258" s="13"/>
+      <c r="E258" s="13"/>
+      <c r="F258" s="13"/>
+    </row>
+    <row r="259" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A259" s="10"/>
+      <c r="B259" s="51" t="s">
         <v>138</v>
       </c>
-      <c r="C249" s="48"/>
-      <c r="D249" s="48"/>
-      <c r="E249" s="48"/>
-      <c r="F249" s="48"/>
-      <c r="G249" s="21"/>
-      <c r="H249" s="21"/>
-      <c r="I249" s="8">
-        <f>G218+H218</f>
-        <v>256.58999999999992</v>
-      </c>
-      <c r="J249" s="8">
-        <f>I249</f>
-        <v>256.58999999999992</v>
-      </c>
-    </row>
-    <row r="250" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A250" s="5"/>
-      <c r="B250" s="49" t="s">
+      <c r="C259" s="51"/>
+      <c r="D259" s="51"/>
+      <c r="E259" s="51"/>
+      <c r="F259" s="51"/>
+      <c r="G259" s="21"/>
+      <c r="H259" s="21"/>
+      <c r="I259" s="8">
+        <f>G228+H228</f>
+        <v>281.58999999999992</v>
+      </c>
+      <c r="J259" s="8">
+        <f>I259</f>
+        <v>281.58999999999992</v>
+      </c>
+    </row>
+    <row r="260" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A260" s="5"/>
+      <c r="B260" s="52" t="s">
         <v>139</v>
       </c>
-      <c r="C250" s="49"/>
-      <c r="D250" s="49"/>
-      <c r="E250" s="49"/>
-      <c r="F250" s="49"/>
-      <c r="I250" s="8">
+      <c r="C260" s="52"/>
+      <c r="D260" s="52"/>
+      <c r="E260" s="52"/>
+      <c r="F260" s="52"/>
+      <c r="I260" s="8">
         <v>300</v>
       </c>
-      <c r="J250" s="8">
+      <c r="J260" s="8">
         <v>200</v>
       </c>
     </row>
-    <row r="251" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A251" s="5"/>
-      <c r="B251" s="49" t="s">
+    <row r="261" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A261" s="5"/>
+      <c r="B261" s="52" t="s">
         <v>140</v>
       </c>
-      <c r="C251" s="49"/>
-      <c r="D251" s="49"/>
-      <c r="E251" s="49"/>
-      <c r="F251" s="49"/>
-      <c r="I251" s="9">
-        <f>I250*I249</f>
-        <v>76976.999999999971</v>
-      </c>
-      <c r="J251" s="9">
-        <f>J250*J249</f>
-        <v>51317.999999999985</v>
-      </c>
-    </row>
-    <row r="252" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A252" s="23"/>
-      <c r="B252" s="50" t="s">
+      <c r="C261" s="52"/>
+      <c r="D261" s="52"/>
+      <c r="E261" s="52"/>
+      <c r="F261" s="52"/>
+      <c r="I261" s="9">
+        <f>I260*I259</f>
+        <v>84476.999999999971</v>
+      </c>
+      <c r="J261" s="9">
+        <f>J260*J259</f>
+        <v>56317.999999999985</v>
+      </c>
+    </row>
+    <row r="262" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A262" s="23"/>
+      <c r="B262" s="53" t="s">
         <v>142</v>
       </c>
-      <c r="C252" s="50"/>
-      <c r="D252" s="50"/>
-      <c r="E252" s="50"/>
-      <c r="F252" s="50"/>
-      <c r="G252" s="24"/>
-      <c r="H252" s="24"/>
-      <c r="I252" s="25"/>
-      <c r="J252" s="25"/>
-    </row>
-    <row r="253" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A253" s="26">
+      <c r="C262" s="53"/>
+      <c r="D262" s="53"/>
+      <c r="E262" s="53"/>
+      <c r="F262" s="53"/>
+      <c r="G262" s="24"/>
+      <c r="H262" s="24"/>
+      <c r="I262" s="25"/>
+      <c r="J262" s="25"/>
+    </row>
+    <row r="263" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A263" s="26">
         <v>45109</v>
       </c>
-      <c r="B253" s="45" t="s">
+      <c r="B263" s="48" t="s">
         <v>141</v>
       </c>
-      <c r="C253" s="45"/>
-      <c r="D253" s="45"/>
-      <c r="E253" s="45"/>
-      <c r="F253" s="45"/>
-      <c r="G253" s="27"/>
-      <c r="H253" s="27"/>
-      <c r="I253" s="28">
+      <c r="C263" s="48"/>
+      <c r="D263" s="48"/>
+      <c r="E263" s="48"/>
+      <c r="F263" s="48"/>
+      <c r="G263" s="27"/>
+      <c r="H263" s="27"/>
+      <c r="I263" s="28">
         <v>10000</v>
       </c>
-      <c r="J253" s="28">
+      <c r="J263" s="28">
         <v>10000</v>
       </c>
     </row>
-    <row r="254" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A254" s="26"/>
-      <c r="B254" s="29"/>
-      <c r="C254" s="29"/>
-      <c r="D254" s="29"/>
-      <c r="E254" s="29"/>
-      <c r="F254" s="29"/>
-      <c r="G254" s="27"/>
-      <c r="H254" s="27"/>
-      <c r="I254" s="30"/>
-      <c r="J254" s="30"/>
-    </row>
-    <row r="255" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A255" s="26"/>
-      <c r="B255" s="29"/>
-      <c r="C255" s="29"/>
-      <c r="D255" s="29"/>
-      <c r="E255" s="29"/>
-      <c r="F255" s="29"/>
-      <c r="G255" s="27"/>
-      <c r="H255" s="27"/>
-      <c r="I255" s="30"/>
-      <c r="J255" s="30"/>
-    </row>
-    <row r="256" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A256" s="26"/>
-      <c r="B256" s="46" t="s">
+    <row r="264" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A264" s="26"/>
+      <c r="B264" s="29"/>
+      <c r="C264" s="29"/>
+      <c r="D264" s="29"/>
+      <c r="E264" s="29"/>
+      <c r="F264" s="29"/>
+      <c r="G264" s="27"/>
+      <c r="H264" s="27"/>
+      <c r="I264" s="30"/>
+      <c r="J264" s="30"/>
+    </row>
+    <row r="265" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A265" s="26"/>
+      <c r="B265" s="29"/>
+      <c r="C265" s="29"/>
+      <c r="D265" s="29"/>
+      <c r="E265" s="29"/>
+      <c r="F265" s="29"/>
+      <c r="G265" s="27"/>
+      <c r="H265" s="27"/>
+      <c r="I265" s="30"/>
+      <c r="J265" s="30"/>
+    </row>
+    <row r="266" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A266" s="26"/>
+      <c r="B266" s="49" t="s">
         <v>144</v>
       </c>
-      <c r="C256" s="46"/>
-      <c r="D256" s="46"/>
-      <c r="E256" s="46"/>
-      <c r="F256" s="46"/>
-      <c r="G256" s="27"/>
-      <c r="H256" s="27"/>
-      <c r="I256" s="31">
-        <f>SUM(I253:I255)</f>
+      <c r="C266" s="49"/>
+      <c r="D266" s="49"/>
+      <c r="E266" s="49"/>
+      <c r="F266" s="49"/>
+      <c r="G266" s="27"/>
+      <c r="H266" s="27"/>
+      <c r="I266" s="31">
+        <f>SUM(I263:I265)</f>
         <v>10000</v>
       </c>
-      <c r="J256" s="31">
-        <f>SUM(J253:J255)</f>
+      <c r="J266" s="31">
+        <f>SUM(J263:J265)</f>
         <v>10000</v>
       </c>
     </row>
-    <row r="257" spans="1:10" ht="33.75" x14ac:dyDescent="0.5">
-      <c r="A257" s="32">
+    <row r="267" spans="1:10" ht="33.75" x14ac:dyDescent="0.5">
+      <c r="A267" s="32">
         <v>45109</v>
       </c>
-      <c r="B257" s="44" t="s">
+      <c r="B267" s="47" t="s">
         <v>143</v>
       </c>
-      <c r="C257" s="44"/>
-      <c r="D257" s="44"/>
-      <c r="E257" s="44"/>
-      <c r="F257" s="44"/>
-      <c r="G257" s="33"/>
-      <c r="H257" s="33"/>
-      <c r="I257" s="34">
-        <f>I251-I256</f>
-        <v>66976.999999999971</v>
-      </c>
-      <c r="J257" s="34">
-        <f>J251-J256</f>
-        <v>41317.999999999985</v>
+      <c r="C267" s="47"/>
+      <c r="D267" s="47"/>
+      <c r="E267" s="47"/>
+      <c r="F267" s="47"/>
+      <c r="G267" s="33"/>
+      <c r="H267" s="33"/>
+      <c r="I267" s="34">
+        <f>I261-I266</f>
+        <v>74476.999999999971</v>
+      </c>
+      <c r="J267" s="34">
+        <f>J261-J266</f>
+        <v>46317.999999999985</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="B257:F257"/>
-    <mergeCell ref="B253:F253"/>
-    <mergeCell ref="B256:F256"/>
-    <mergeCell ref="A219:F219"/>
-    <mergeCell ref="A218:F218"/>
-    <mergeCell ref="A220:F220"/>
-    <mergeCell ref="A221:F221"/>
-    <mergeCell ref="B227:F227"/>
-    <mergeCell ref="B228:F228"/>
-    <mergeCell ref="B249:F249"/>
-    <mergeCell ref="B250:F250"/>
-    <mergeCell ref="B251:F251"/>
-    <mergeCell ref="B252:F252"/>
-    <mergeCell ref="G221:H221"/>
+    <mergeCell ref="B267:F267"/>
+    <mergeCell ref="B263:F263"/>
+    <mergeCell ref="B266:F266"/>
+    <mergeCell ref="A229:F229"/>
+    <mergeCell ref="A228:F228"/>
     <mergeCell ref="A230:F230"/>
-    <mergeCell ref="G230:H230"/>
-    <mergeCell ref="B222:F222"/>
-    <mergeCell ref="B223:F223"/>
-    <mergeCell ref="B229:F229"/>
-    <mergeCell ref="G223:H223"/>
-    <mergeCell ref="G224:H224"/>
-    <mergeCell ref="G229:H229"/>
-    <mergeCell ref="G226:H226"/>
-    <mergeCell ref="G227:H227"/>
-    <mergeCell ref="G228:H228"/>
-    <mergeCell ref="G225:H225"/>
-    <mergeCell ref="B225:F225"/>
-    <mergeCell ref="B224:F224"/>
-    <mergeCell ref="B226:F226"/>
+    <mergeCell ref="A231:F231"/>
+    <mergeCell ref="B237:F237"/>
+    <mergeCell ref="B238:F238"/>
+    <mergeCell ref="B259:F259"/>
+    <mergeCell ref="B260:F260"/>
+    <mergeCell ref="B261:F261"/>
+    <mergeCell ref="B262:F262"/>
+    <mergeCell ref="G231:H231"/>
+    <mergeCell ref="A240:F240"/>
+    <mergeCell ref="G240:H240"/>
+    <mergeCell ref="B232:F232"/>
+    <mergeCell ref="B233:F233"/>
+    <mergeCell ref="B239:F239"/>
+    <mergeCell ref="G233:H233"/>
+    <mergeCell ref="G234:H234"/>
+    <mergeCell ref="G239:H239"/>
+    <mergeCell ref="G236:H236"/>
+    <mergeCell ref="G237:H237"/>
+    <mergeCell ref="G238:H238"/>
+    <mergeCell ref="G235:H235"/>
+    <mergeCell ref="B235:F235"/>
+    <mergeCell ref="B234:F234"/>
+    <mergeCell ref="B236:F236"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -6125,10 +6390,189 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="17.7109375" customWidth="1"/>
+    <col min="3" max="3" width="69.5703125" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" style="35" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.140625" style="35" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" style="35"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>234</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="35" t="s">
+        <v>232</v>
+      </c>
+      <c r="E1" s="35" t="s">
+        <v>237</v>
+      </c>
+      <c r="F1" s="35" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>235</v>
+      </c>
+      <c r="C2" t="s">
+        <v>236</v>
+      </c>
+      <c r="D2" s="35">
+        <v>2</v>
+      </c>
+      <c r="E2" s="36" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>240</v>
+      </c>
+      <c r="C3" t="s">
+        <v>239</v>
+      </c>
+      <c r="D3" s="35">
+        <v>1</v>
+      </c>
+      <c r="E3" s="36" t="s">
+        <v>238</v>
+      </c>
+      <c r="F3" s="35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>243</v>
+      </c>
+      <c r="C4" t="s">
+        <v>242</v>
+      </c>
+      <c r="E4" s="37" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>245</v>
+      </c>
+      <c r="C5" t="s">
+        <v>244</v>
+      </c>
+      <c r="E5" s="37" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>235</v>
+      </c>
+      <c r="C6" t="s">
+        <v>246</v>
+      </c>
+      <c r="D6" s="35">
+        <v>1</v>
+      </c>
+      <c r="E6" s="36" t="s">
+        <v>238</v>
+      </c>
+      <c r="F6" s="35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>110</v>
+      </c>
+      <c r="C7" t="s">
+        <v>252</v>
+      </c>
+      <c r="E7" s="37" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>254</v>
+      </c>
+      <c r="C8" t="s">
+        <v>253</v>
+      </c>
+      <c r="E8" s="36" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>256</v>
+      </c>
+      <c r="E9" s="37" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>258</v>
+      </c>
+      <c r="E10" s="37" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>262</v>
+      </c>
+      <c r="E11" s="37" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>260</v>
+      </c>
+      <c r="E12" s="36" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>259</v>
+      </c>
+      <c r="E13" s="36" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>261</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D98"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D95" sqref="D95"/>
     </sheetView>
   </sheetViews>
@@ -6155,12 +6599,12 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="51" t="s">
+      <c r="A2" s="54" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="51"/>
-      <c r="C2" s="51"/>
-      <c r="D2" s="51"/>
+      <c r="B2" s="54"/>
+      <c r="C2" s="54"/>
+      <c r="D2" s="54"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
@@ -6463,12 +6907,12 @@
       <c r="D30" s="6"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="52" t="s">
+      <c r="A31" s="55" t="s">
         <v>43</v>
       </c>
-      <c r="B31" s="52"/>
-      <c r="C31" s="52"/>
-      <c r="D31" s="52"/>
+      <c r="B31" s="55"/>
+      <c r="C31" s="55"/>
+      <c r="D31" s="55"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
@@ -7097,10 +7541,10 @@
       <c r="D97" s="6"/>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A98" s="52"/>
-      <c r="B98" s="52"/>
-      <c r="C98" s="52"/>
-      <c r="D98" s="52"/>
+      <c r="A98" s="55"/>
+      <c r="B98" s="55"/>
+      <c r="C98" s="55"/>
+      <c r="D98" s="55"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
Se versiona el código
</commit_message>
<xml_diff>
--- a/Documents/Actividades realizadas/ActividadesN.xlsx
+++ b/Documents/Actividades realizadas/ActividadesN.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="555" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="561" uniqueCount="265">
   <si>
     <t>Descripción</t>
   </si>
@@ -821,6 +821,12 @@
   </si>
   <si>
     <t>Rediseñar impresión de ticket de taller notas de taller</t>
+  </si>
+  <si>
+    <t>Cerrar la ventana del cliente cuando se agrega o se actualiza</t>
+  </si>
+  <si>
+    <t>Agregar atajo de inventario de producto desde la consulta</t>
   </si>
 </sst>
 </file>
@@ -1036,6 +1042,30 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="44" fontId="3" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1051,9 +1081,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1062,27 +1089,6 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1398,7 +1404,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1406,11 +1412,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K267"/>
+  <dimension ref="A1:K272"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A214" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G222" sqref="G222:G223"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A216" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D226" sqref="D226"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5848,13 +5854,33 @@
     </row>
     <row r="224" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A224" s="5"/>
-      <c r="E224" s="2"/>
-      <c r="F224" s="2"/>
+      <c r="D224" t="s">
+        <v>263</v>
+      </c>
+      <c r="E224" s="2">
+        <v>0.375</v>
+      </c>
+      <c r="F224" s="2">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="G224" s="15">
+        <v>1</v>
+      </c>
     </row>
     <row r="225" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A225" s="5"/>
-      <c r="E225" s="2"/>
-      <c r="F225" s="2"/>
+      <c r="D225" t="s">
+        <v>264</v>
+      </c>
+      <c r="E225" s="2">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="F225" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="G225" s="15">
+        <v>2</v>
+      </c>
     </row>
     <row r="226" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A226" s="5"/>
@@ -5867,233 +5893,218 @@
       <c r="F227" s="2"/>
     </row>
     <row r="228" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A228" s="50" t="s">
+      <c r="A228" s="5"/>
+      <c r="E228" s="2"/>
+      <c r="F228" s="2"/>
+    </row>
+    <row r="229" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A229" s="5"/>
+      <c r="E229" s="2"/>
+      <c r="F229" s="2"/>
+    </row>
+    <row r="230" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A230" s="5"/>
+      <c r="E230" s="2"/>
+      <c r="F230" s="2"/>
+    </row>
+    <row r="231" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A231" s="5"/>
+      <c r="E231" s="2"/>
+      <c r="F231" s="2"/>
+    </row>
+    <row r="232" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A232" s="5"/>
+      <c r="E232" s="2"/>
+      <c r="F232" s="2"/>
+    </row>
+    <row r="233" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A233" s="41" t="s">
         <v>165</v>
       </c>
-      <c r="B228" s="50"/>
-      <c r="C228" s="50"/>
-      <c r="D228" s="50"/>
-      <c r="E228" s="50"/>
-      <c r="F228" s="50"/>
-      <c r="G228" s="17">
-        <f>SUM(G2:G227)</f>
-        <v>238.78999999999994</v>
-      </c>
-      <c r="H228" s="17">
-        <f>SUM(H2:H227)</f>
+      <c r="B233" s="41"/>
+      <c r="C233" s="41"/>
+      <c r="D233" s="41"/>
+      <c r="E233" s="41"/>
+      <c r="F233" s="41"/>
+      <c r="G233" s="17">
+        <f>SUM(G2:G232)</f>
+        <v>241.78999999999994</v>
+      </c>
+      <c r="H233" s="17">
+        <f>SUM(H2:H232)</f>
         <v>42.8</v>
       </c>
     </row>
-    <row r="229" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A229" s="50" t="s">
+    <row r="234" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A234" s="41" t="s">
         <v>139</v>
       </c>
-      <c r="B229" s="50"/>
-      <c r="C229" s="50"/>
-      <c r="D229" s="50"/>
-      <c r="E229" s="50"/>
-      <c r="F229" s="50"/>
-      <c r="G229" s="17">
+      <c r="B234" s="41"/>
+      <c r="C234" s="41"/>
+      <c r="D234" s="41"/>
+      <c r="E234" s="41"/>
+      <c r="F234" s="41"/>
+      <c r="G234" s="17">
         <v>200</v>
       </c>
-      <c r="H229" s="17">
+      <c r="H234" s="17">
         <v>300</v>
       </c>
     </row>
-    <row r="230" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A230" s="50" t="s">
+    <row r="235" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A235" s="41" t="s">
         <v>166</v>
       </c>
-      <c r="B230" s="50"/>
-      <c r="C230" s="50"/>
-      <c r="D230" s="50"/>
-      <c r="E230" s="50"/>
-      <c r="F230" s="50"/>
-      <c r="G230" s="18">
-        <f>G229*G228</f>
-        <v>47757.999999999985</v>
-      </c>
-      <c r="H230" s="19">
-        <f>H229*H228</f>
+      <c r="B235" s="41"/>
+      <c r="C235" s="41"/>
+      <c r="D235" s="41"/>
+      <c r="E235" s="41"/>
+      <c r="F235" s="41"/>
+      <c r="G235" s="18">
+        <f>G234*G233</f>
+        <v>48357.999999999985</v>
+      </c>
+      <c r="H235" s="19">
+        <f>H234*H233</f>
         <v>12840</v>
       </c>
-      <c r="J230">
+      <c r="J235">
         <v>-500</v>
       </c>
     </row>
-    <row r="231" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A231" s="50" t="s">
+    <row r="236" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A236" s="41" t="s">
         <v>140</v>
       </c>
-      <c r="B231" s="50"/>
-      <c r="C231" s="50"/>
-      <c r="D231" s="50"/>
-      <c r="E231" s="50"/>
-      <c r="F231" s="50"/>
-      <c r="G231" s="38">
-        <f>G230+H230</f>
-        <v>60597.999999999985</v>
-      </c>
-      <c r="H231" s="38"/>
-    </row>
-    <row r="232" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A232" s="11"/>
-      <c r="B232" s="41" t="s">
+      <c r="B236" s="41"/>
+      <c r="C236" s="41"/>
+      <c r="D236" s="41"/>
+      <c r="E236" s="41"/>
+      <c r="F236" s="41"/>
+      <c r="G236" s="46">
+        <f>G235+H235</f>
+        <v>61197.999999999985</v>
+      </c>
+      <c r="H236" s="46"/>
+    </row>
+    <row r="237" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A237" s="11"/>
+      <c r="B237" s="49" t="s">
         <v>142</v>
       </c>
-      <c r="C232" s="41"/>
-      <c r="D232" s="41"/>
-      <c r="E232" s="41"/>
-      <c r="F232" s="41"/>
-      <c r="G232" s="22"/>
-    </row>
-    <row r="233" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A233" s="12">
+      <c r="C237" s="49"/>
+      <c r="D237" s="49"/>
+      <c r="E237" s="49"/>
+      <c r="F237" s="49"/>
+      <c r="G237" s="22"/>
+    </row>
+    <row r="238" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A238" s="12">
         <v>45109</v>
       </c>
-      <c r="B233" s="42" t="s">
+      <c r="B238" s="50" t="s">
         <v>141</v>
       </c>
-      <c r="C233" s="42"/>
-      <c r="D233" s="42"/>
-      <c r="E233" s="42"/>
-      <c r="F233" s="42"/>
-      <c r="G233" s="44">
+      <c r="C238" s="50"/>
+      <c r="D238" s="50"/>
+      <c r="E238" s="50"/>
+      <c r="F238" s="50"/>
+      <c r="G238" s="51">
         <v>10000</v>
       </c>
-      <c r="H233" s="44"/>
-    </row>
-    <row r="234" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A234" s="12"/>
-      <c r="B234" s="46" t="s">
-        <v>178</v>
-      </c>
-      <c r="C234" s="46"/>
-      <c r="D234" s="46"/>
-      <c r="E234" s="46"/>
-      <c r="F234" s="46"/>
-      <c r="G234" s="44">
-        <v>5000</v>
-      </c>
-      <c r="H234" s="44"/>
-    </row>
-    <row r="235" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A235" s="12">
-        <v>45278</v>
-      </c>
-      <c r="B235" s="43" t="s">
-        <v>178</v>
-      </c>
-      <c r="C235" s="43"/>
-      <c r="D235" s="43"/>
-      <c r="E235" s="43"/>
-      <c r="F235" s="43"/>
-      <c r="G235" s="44">
-        <v>9800</v>
-      </c>
-      <c r="H235" s="44"/>
-    </row>
-    <row r="236" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A236" s="12"/>
-      <c r="B236" s="43"/>
-      <c r="C236" s="43"/>
-      <c r="D236" s="43"/>
-      <c r="E236" s="43"/>
-      <c r="F236" s="43"/>
-      <c r="G236" s="45"/>
-      <c r="H236" s="45"/>
-    </row>
-    <row r="237" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A237" s="12"/>
-      <c r="B237" s="43"/>
-      <c r="C237" s="43"/>
-      <c r="D237" s="43"/>
-      <c r="E237" s="43"/>
-      <c r="F237" s="43"/>
-      <c r="G237" s="45"/>
-      <c r="H237" s="45"/>
-    </row>
-    <row r="238" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A238" s="12"/>
-      <c r="B238" s="43"/>
-      <c r="C238" s="43"/>
-      <c r="D238" s="43"/>
-      <c r="E238" s="43"/>
-      <c r="F238" s="43"/>
-      <c r="G238" s="45"/>
-      <c r="H238" s="45"/>
+      <c r="H238" s="51"/>
     </row>
     <row r="239" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A239" s="12"/>
-      <c r="B239" s="43" t="s">
+      <c r="B239" s="53" t="s">
+        <v>178</v>
+      </c>
+      <c r="C239" s="53"/>
+      <c r="D239" s="53"/>
+      <c r="E239" s="53"/>
+      <c r="F239" s="53"/>
+      <c r="G239" s="51">
+        <v>5000</v>
+      </c>
+      <c r="H239" s="51"/>
+    </row>
+    <row r="240" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A240" s="12">
+        <v>45278</v>
+      </c>
+      <c r="B240" s="42" t="s">
+        <v>178</v>
+      </c>
+      <c r="C240" s="42"/>
+      <c r="D240" s="42"/>
+      <c r="E240" s="42"/>
+      <c r="F240" s="42"/>
+      <c r="G240" s="51">
+        <v>9800</v>
+      </c>
+      <c r="H240" s="51"/>
+    </row>
+    <row r="241" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A241" s="12"/>
+      <c r="B241" s="42"/>
+      <c r="C241" s="42"/>
+      <c r="D241" s="42"/>
+      <c r="E241" s="42"/>
+      <c r="F241" s="42"/>
+      <c r="G241" s="52"/>
+      <c r="H241" s="52"/>
+    </row>
+    <row r="242" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A242" s="12"/>
+      <c r="B242" s="42"/>
+      <c r="C242" s="42"/>
+      <c r="D242" s="42"/>
+      <c r="E242" s="42"/>
+      <c r="F242" s="42"/>
+      <c r="G242" s="52"/>
+      <c r="H242" s="52"/>
+    </row>
+    <row r="243" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A243" s="12"/>
+      <c r="B243" s="42"/>
+      <c r="C243" s="42"/>
+      <c r="D243" s="42"/>
+      <c r="E243" s="42"/>
+      <c r="F243" s="42"/>
+      <c r="G243" s="52"/>
+      <c r="H243" s="52"/>
+    </row>
+    <row r="244" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A244" s="12"/>
+      <c r="B244" s="42" t="s">
         <v>144</v>
       </c>
-      <c r="C239" s="43"/>
-      <c r="D239" s="43"/>
-      <c r="E239" s="43"/>
-      <c r="F239" s="43"/>
-      <c r="G239" s="44">
-        <f>SUM(G233:H238)</f>
+      <c r="C244" s="42"/>
+      <c r="D244" s="42"/>
+      <c r="E244" s="42"/>
+      <c r="F244" s="42"/>
+      <c r="G244" s="51">
+        <f>SUM(G238:H243)</f>
         <v>24800</v>
       </c>
-      <c r="H239" s="44"/>
-    </row>
-    <row r="240" spans="1:10" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A240" s="39" t="s">
+      <c r="H244" s="51"/>
+    </row>
+    <row r="245" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+      <c r="A245" s="47" t="s">
         <v>143</v>
       </c>
-      <c r="B240" s="39"/>
-      <c r="C240" s="39"/>
-      <c r="D240" s="39"/>
-      <c r="E240" s="39"/>
-      <c r="F240" s="39"/>
-      <c r="G240" s="40">
-        <f>G231-G239</f>
-        <v>35797.999999999985</v>
-      </c>
-      <c r="H240" s="40"/>
-    </row>
-    <row r="241" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A241" s="12"/>
-      <c r="B241" s="13"/>
-      <c r="C241" s="13"/>
-      <c r="D241" s="13"/>
-      <c r="E241" s="13"/>
-      <c r="F241" s="13"/>
-    </row>
-    <row r="242" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A242" s="12"/>
-      <c r="B242" s="13"/>
-      <c r="C242" s="13"/>
-      <c r="D242" s="13"/>
-      <c r="E242" s="13"/>
-      <c r="F242" s="13"/>
-    </row>
-    <row r="243" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A243" s="12"/>
-      <c r="B243" s="13"/>
-      <c r="C243" s="13"/>
-      <c r="D243" s="13"/>
-      <c r="E243" s="13"/>
-      <c r="F243" s="13"/>
-    </row>
-    <row r="244" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A244" s="12"/>
-      <c r="B244" s="13"/>
-      <c r="C244" s="13"/>
-      <c r="D244" s="13"/>
-      <c r="E244" s="13"/>
-      <c r="F244" s="13"/>
-    </row>
-    <row r="245" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A245" s="12"/>
-      <c r="B245" s="13"/>
-      <c r="C245" s="13"/>
-      <c r="D245" s="13"/>
-      <c r="E245" s="13"/>
-      <c r="F245" s="13"/>
-    </row>
-    <row r="246" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B245" s="47"/>
+      <c r="C245" s="47"/>
+      <c r="D245" s="47"/>
+      <c r="E245" s="47"/>
+      <c r="F245" s="47"/>
+      <c r="G245" s="48">
+        <f>G236-G244</f>
+        <v>36397.999999999985</v>
+      </c>
+      <c r="H245" s="48"/>
+    </row>
+    <row r="246" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A246" s="12"/>
       <c r="B246" s="13"/>
       <c r="C246" s="13"/>
@@ -6101,7 +6112,7 @@
       <c r="E246" s="13"/>
       <c r="F246" s="13"/>
     </row>
-    <row r="247" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A247" s="12"/>
       <c r="B247" s="13"/>
       <c r="C247" s="13"/>
@@ -6109,7 +6120,7 @@
       <c r="E247" s="13"/>
       <c r="F247" s="13"/>
     </row>
-    <row r="248" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A248" s="12"/>
       <c r="B248" s="13"/>
       <c r="C248" s="13"/>
@@ -6117,7 +6128,7 @@
       <c r="E248" s="13"/>
       <c r="F248" s="13"/>
     </row>
-    <row r="249" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A249" s="12"/>
       <c r="B249" s="13"/>
       <c r="C249" s="13"/>
@@ -6125,7 +6136,7 @@
       <c r="E249" s="13"/>
       <c r="F249" s="13"/>
     </row>
-    <row r="250" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A250" s="12"/>
       <c r="B250" s="13"/>
       <c r="C250" s="13"/>
@@ -6133,7 +6144,7 @@
       <c r="E250" s="13"/>
       <c r="F250" s="13"/>
     </row>
-    <row r="251" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A251" s="12"/>
       <c r="B251" s="13"/>
       <c r="C251" s="13"/>
@@ -6141,7 +6152,7 @@
       <c r="E251" s="13"/>
       <c r="F251" s="13"/>
     </row>
-    <row r="252" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A252" s="12"/>
       <c r="B252" s="13"/>
       <c r="C252" s="13"/>
@@ -6149,7 +6160,7 @@
       <c r="E252" s="13"/>
       <c r="F252" s="13"/>
     </row>
-    <row r="253" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A253" s="12"/>
       <c r="B253" s="13"/>
       <c r="C253" s="13"/>
@@ -6157,7 +6168,7 @@
       <c r="E253" s="13"/>
       <c r="F253" s="13"/>
     </row>
-    <row r="254" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A254" s="12"/>
       <c r="B254" s="13"/>
       <c r="C254" s="13"/>
@@ -6165,7 +6176,7 @@
       <c r="E254" s="13"/>
       <c r="F254" s="13"/>
     </row>
-    <row r="255" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A255" s="12"/>
       <c r="B255" s="13"/>
       <c r="C255" s="13"/>
@@ -6173,7 +6184,7 @@
       <c r="E255" s="13"/>
       <c r="F255" s="13"/>
     </row>
-    <row r="256" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A256" s="12"/>
       <c r="B256" s="13"/>
       <c r="C256" s="13"/>
@@ -6198,190 +6209,230 @@
       <c r="F258" s="13"/>
     </row>
     <row r="259" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A259" s="10"/>
-      <c r="B259" s="51" t="s">
+      <c r="A259" s="12"/>
+      <c r="B259" s="13"/>
+      <c r="C259" s="13"/>
+      <c r="D259" s="13"/>
+      <c r="E259" s="13"/>
+      <c r="F259" s="13"/>
+    </row>
+    <row r="260" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A260" s="12"/>
+      <c r="B260" s="13"/>
+      <c r="C260" s="13"/>
+      <c r="D260" s="13"/>
+      <c r="E260" s="13"/>
+      <c r="F260" s="13"/>
+    </row>
+    <row r="261" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A261" s="12"/>
+      <c r="B261" s="13"/>
+      <c r="C261" s="13"/>
+      <c r="D261" s="13"/>
+      <c r="E261" s="13"/>
+      <c r="F261" s="13"/>
+    </row>
+    <row r="262" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A262" s="12"/>
+      <c r="B262" s="13"/>
+      <c r="C262" s="13"/>
+      <c r="D262" s="13"/>
+      <c r="E262" s="13"/>
+      <c r="F262" s="13"/>
+    </row>
+    <row r="263" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A263" s="12"/>
+      <c r="B263" s="13"/>
+      <c r="C263" s="13"/>
+      <c r="D263" s="13"/>
+      <c r="E263" s="13"/>
+      <c r="F263" s="13"/>
+    </row>
+    <row r="264" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A264" s="10"/>
+      <c r="B264" s="43" t="s">
         <v>138</v>
       </c>
-      <c r="C259" s="51"/>
-      <c r="D259" s="51"/>
-      <c r="E259" s="51"/>
-      <c r="F259" s="51"/>
-      <c r="G259" s="21"/>
-      <c r="H259" s="21"/>
-      <c r="I259" s="8">
-        <f>G228+H228</f>
-        <v>281.58999999999992</v>
-      </c>
-      <c r="J259" s="8">
-        <f>I259</f>
-        <v>281.58999999999992</v>
-      </c>
-    </row>
-    <row r="260" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A260" s="5"/>
-      <c r="B260" s="52" t="s">
+      <c r="C264" s="43"/>
+      <c r="D264" s="43"/>
+      <c r="E264" s="43"/>
+      <c r="F264" s="43"/>
+      <c r="G264" s="21"/>
+      <c r="H264" s="21"/>
+      <c r="I264" s="8">
+        <f>G233+H233</f>
+        <v>284.58999999999992</v>
+      </c>
+      <c r="J264" s="8">
+        <f>I264</f>
+        <v>284.58999999999992</v>
+      </c>
+    </row>
+    <row r="265" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A265" s="5"/>
+      <c r="B265" s="44" t="s">
         <v>139</v>
       </c>
-      <c r="C260" s="52"/>
-      <c r="D260" s="52"/>
-      <c r="E260" s="52"/>
-      <c r="F260" s="52"/>
-      <c r="I260" s="8">
+      <c r="C265" s="44"/>
+      <c r="D265" s="44"/>
+      <c r="E265" s="44"/>
+      <c r="F265" s="44"/>
+      <c r="I265" s="8">
         <v>300</v>
       </c>
-      <c r="J260" s="8">
+      <c r="J265" s="8">
         <v>200</v>
       </c>
     </row>
-    <row r="261" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A261" s="5"/>
-      <c r="B261" s="52" t="s">
+    <row r="266" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A266" s="5"/>
+      <c r="B266" s="44" t="s">
         <v>140</v>
       </c>
-      <c r="C261" s="52"/>
-      <c r="D261" s="52"/>
-      <c r="E261" s="52"/>
-      <c r="F261" s="52"/>
-      <c r="I261" s="9">
-        <f>I260*I259</f>
-        <v>84476.999999999971</v>
-      </c>
-      <c r="J261" s="9">
-        <f>J260*J259</f>
-        <v>56317.999999999985</v>
-      </c>
-    </row>
-    <row r="262" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A262" s="23"/>
-      <c r="B262" s="53" t="s">
+      <c r="C266" s="44"/>
+      <c r="D266" s="44"/>
+      <c r="E266" s="44"/>
+      <c r="F266" s="44"/>
+      <c r="I266" s="9">
+        <f>I265*I264</f>
+        <v>85376.999999999971</v>
+      </c>
+      <c r="J266" s="9">
+        <f>J265*J264</f>
+        <v>56917.999999999985</v>
+      </c>
+    </row>
+    <row r="267" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A267" s="23"/>
+      <c r="B267" s="45" t="s">
         <v>142</v>
       </c>
-      <c r="C262" s="53"/>
-      <c r="D262" s="53"/>
-      <c r="E262" s="53"/>
-      <c r="F262" s="53"/>
-      <c r="G262" s="24"/>
-      <c r="H262" s="24"/>
-      <c r="I262" s="25"/>
-      <c r="J262" s="25"/>
-    </row>
-    <row r="263" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A263" s="26">
+      <c r="C267" s="45"/>
+      <c r="D267" s="45"/>
+      <c r="E267" s="45"/>
+      <c r="F267" s="45"/>
+      <c r="G267" s="24"/>
+      <c r="H267" s="24"/>
+      <c r="I267" s="25"/>
+      <c r="J267" s="25"/>
+    </row>
+    <row r="268" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A268" s="26">
         <v>45109</v>
       </c>
-      <c r="B263" s="48" t="s">
+      <c r="B268" s="39" t="s">
         <v>141</v>
       </c>
-      <c r="C263" s="48"/>
-      <c r="D263" s="48"/>
-      <c r="E263" s="48"/>
-      <c r="F263" s="48"/>
-      <c r="G263" s="27"/>
-      <c r="H263" s="27"/>
-      <c r="I263" s="28">
+      <c r="C268" s="39"/>
+      <c r="D268" s="39"/>
+      <c r="E268" s="39"/>
+      <c r="F268" s="39"/>
+      <c r="G268" s="27"/>
+      <c r="H268" s="27"/>
+      <c r="I268" s="28">
         <v>10000</v>
       </c>
-      <c r="J263" s="28">
+      <c r="J268" s="28">
         <v>10000</v>
       </c>
     </row>
-    <row r="264" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A264" s="26"/>
-      <c r="B264" s="29"/>
-      <c r="C264" s="29"/>
-      <c r="D264" s="29"/>
-      <c r="E264" s="29"/>
-      <c r="F264" s="29"/>
-      <c r="G264" s="27"/>
-      <c r="H264" s="27"/>
-      <c r="I264" s="30"/>
-      <c r="J264" s="30"/>
-    </row>
-    <row r="265" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A265" s="26"/>
-      <c r="B265" s="29"/>
-      <c r="C265" s="29"/>
-      <c r="D265" s="29"/>
-      <c r="E265" s="29"/>
-      <c r="F265" s="29"/>
-      <c r="G265" s="27"/>
-      <c r="H265" s="27"/>
-      <c r="I265" s="30"/>
-      <c r="J265" s="30"/>
-    </row>
-    <row r="266" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A266" s="26"/>
-      <c r="B266" s="49" t="s">
+    <row r="269" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A269" s="26"/>
+      <c r="B269" s="29"/>
+      <c r="C269" s="29"/>
+      <c r="D269" s="29"/>
+      <c r="E269" s="29"/>
+      <c r="F269" s="29"/>
+      <c r="G269" s="27"/>
+      <c r="H269" s="27"/>
+      <c r="I269" s="30"/>
+      <c r="J269" s="30"/>
+    </row>
+    <row r="270" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A270" s="26"/>
+      <c r="B270" s="29"/>
+      <c r="C270" s="29"/>
+      <c r="D270" s="29"/>
+      <c r="E270" s="29"/>
+      <c r="F270" s="29"/>
+      <c r="G270" s="27"/>
+      <c r="H270" s="27"/>
+      <c r="I270" s="30"/>
+      <c r="J270" s="30"/>
+    </row>
+    <row r="271" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A271" s="26"/>
+      <c r="B271" s="40" t="s">
         <v>144</v>
       </c>
-      <c r="C266" s="49"/>
-      <c r="D266" s="49"/>
-      <c r="E266" s="49"/>
-      <c r="F266" s="49"/>
-      <c r="G266" s="27"/>
-      <c r="H266" s="27"/>
-      <c r="I266" s="31">
-        <f>SUM(I263:I265)</f>
+      <c r="C271" s="40"/>
+      <c r="D271" s="40"/>
+      <c r="E271" s="40"/>
+      <c r="F271" s="40"/>
+      <c r="G271" s="27"/>
+      <c r="H271" s="27"/>
+      <c r="I271" s="31">
+        <f>SUM(I268:I270)</f>
         <v>10000</v>
       </c>
-      <c r="J266" s="31">
-        <f>SUM(J263:J265)</f>
+      <c r="J271" s="31">
+        <f>SUM(J268:J270)</f>
         <v>10000</v>
       </c>
     </row>
-    <row r="267" spans="1:10" ht="33.75" x14ac:dyDescent="0.5">
-      <c r="A267" s="32">
+    <row r="272" spans="1:10" ht="33.75" x14ac:dyDescent="0.5">
+      <c r="A272" s="32">
         <v>45109</v>
       </c>
-      <c r="B267" s="47" t="s">
+      <c r="B272" s="38" t="s">
         <v>143</v>
       </c>
-      <c r="C267" s="47"/>
-      <c r="D267" s="47"/>
-      <c r="E267" s="47"/>
-      <c r="F267" s="47"/>
-      <c r="G267" s="33"/>
-      <c r="H267" s="33"/>
-      <c r="I267" s="34">
-        <f>I261-I266</f>
-        <v>74476.999999999971</v>
-      </c>
-      <c r="J267" s="34">
-        <f>J261-J266</f>
-        <v>46317.999999999985</v>
+      <c r="C272" s="38"/>
+      <c r="D272" s="38"/>
+      <c r="E272" s="38"/>
+      <c r="F272" s="38"/>
+      <c r="G272" s="33"/>
+      <c r="H272" s="33"/>
+      <c r="I272" s="34">
+        <f>I266-I271</f>
+        <v>75376.999999999971</v>
+      </c>
+      <c r="J272" s="34">
+        <f>J266-J271</f>
+        <v>46917.999999999985</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="B267:F267"/>
-    <mergeCell ref="B263:F263"/>
-    <mergeCell ref="B266:F266"/>
-    <mergeCell ref="A229:F229"/>
-    <mergeCell ref="A228:F228"/>
-    <mergeCell ref="A230:F230"/>
-    <mergeCell ref="A231:F231"/>
+    <mergeCell ref="G236:H236"/>
+    <mergeCell ref="A245:F245"/>
+    <mergeCell ref="G245:H245"/>
     <mergeCell ref="B237:F237"/>
     <mergeCell ref="B238:F238"/>
-    <mergeCell ref="B259:F259"/>
-    <mergeCell ref="B260:F260"/>
-    <mergeCell ref="B261:F261"/>
-    <mergeCell ref="B262:F262"/>
-    <mergeCell ref="G231:H231"/>
-    <mergeCell ref="A240:F240"/>
+    <mergeCell ref="B244:F244"/>
+    <mergeCell ref="G238:H238"/>
+    <mergeCell ref="G239:H239"/>
+    <mergeCell ref="G244:H244"/>
+    <mergeCell ref="G241:H241"/>
+    <mergeCell ref="G242:H242"/>
+    <mergeCell ref="G243:H243"/>
     <mergeCell ref="G240:H240"/>
-    <mergeCell ref="B232:F232"/>
-    <mergeCell ref="B233:F233"/>
+    <mergeCell ref="B240:F240"/>
     <mergeCell ref="B239:F239"/>
-    <mergeCell ref="G233:H233"/>
-    <mergeCell ref="G234:H234"/>
-    <mergeCell ref="G239:H239"/>
-    <mergeCell ref="G236:H236"/>
-    <mergeCell ref="G237:H237"/>
-    <mergeCell ref="G238:H238"/>
-    <mergeCell ref="G235:H235"/>
-    <mergeCell ref="B235:F235"/>
-    <mergeCell ref="B234:F234"/>
-    <mergeCell ref="B236:F236"/>
+    <mergeCell ref="B241:F241"/>
+    <mergeCell ref="B272:F272"/>
+    <mergeCell ref="B268:F268"/>
+    <mergeCell ref="B271:F271"/>
+    <mergeCell ref="A234:F234"/>
+    <mergeCell ref="A233:F233"/>
+    <mergeCell ref="A235:F235"/>
+    <mergeCell ref="A236:F236"/>
+    <mergeCell ref="B242:F242"/>
+    <mergeCell ref="B243:F243"/>
+    <mergeCell ref="B264:F264"/>
+    <mergeCell ref="B265:F265"/>
+    <mergeCell ref="B266:F266"/>
+    <mergeCell ref="B267:F267"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -6390,10 +6441,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C15" sqref="C15:C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6560,6 +6611,22 @@
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
         <v>261</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
+        <v>263</v>
+      </c>
+      <c r="E15" s="36" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>264</v>
+      </c>
+      <c r="E16" s="36" t="s">
+        <v>238</v>
       </c>
     </row>
   </sheetData>

</xml_diff>